<commit_message>
Final branch cleanup before merge
</commit_message>
<xml_diff>
--- a/resources/wwtp_classes.xlsx
+++ b/resources/wwtp_classes.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -813,7 +813,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>

</xml_diff>